<commit_message>
actualizado con envío a facebook y telegram
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -18,7 +18,7 @@
     <sheet name="Tractocamiones" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$B$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$B$27</definedName>
   </definedNames>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6874" uniqueCount="3960">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6876" uniqueCount="3962">
   <si>
     <t>contact_name</t>
   </si>
@@ -11910,6 +11910,12 @@
   </si>
   <si>
     <t>contact_name_2</t>
+  </si>
+  <si>
+    <t>Transportadores&amp;nbsp;&amp;nbsp;Colombia</t>
+  </si>
+  <si>
+    <t>VIAJES CONDUCTORES COLOMB</t>
   </si>
 </sst>
 </file>
@@ -12320,10 +12326,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12461,7 +12467,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -12469,7 +12475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -12477,7 +12483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>3953</v>
       </c>
@@ -12485,7 +12491,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3958</v>
       </c>
@@ -12493,15 +12499,16 @@
         <v>3950</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3957</v>
       </c>
       <c r="B21" t="s">
         <v>3949</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -12509,7 +12516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3948</v>
       </c>
@@ -12517,72 +12524,80 @@
         <v>3948</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>3954</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3952</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>3955</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3951</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>3956</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3947</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>3961</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>3961</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>2801</v>
       </c>
-      <c r="B24" t="s">
-        <v>2801</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>3954</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>3952</v>
-      </c>
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>3955</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>3951</v>
-      </c>
-      <c r="B30" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>3956</v>
-      </c>
-      <c r="B31" t="s">
-        <v>3947</v>
+      <c r="B32" t="s">
+        <v>3960</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B28">
+  <autoFilter ref="A1:B27">
     <sortState ref="A2:B31">
       <sortCondition ref="A2:A31"/>
     </sortState>

</xml_diff>